<commit_message>
Funcionando, mas não inclui comentários só no teste.py
</commit_message>
<xml_diff>
--- a/priorizadas_semana.xlsx
+++ b/priorizadas_semana.xlsx
@@ -19664,7 +19664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19685,30 +19685,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Proprietário</t>
+          <t>Priorizada</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Priorizada</t>
+          <t>Atualizado em</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Atualizado em</t>
+          <t>Data_priorizado</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Data_priorizado</t>
+          <t>hora_priorizado</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>hora_priorizado</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Município</t>
         </is>
@@ -19723,30 +19718,25 @@
           <t>[Petrolina-PE][Regulação] - Permitir selecionar lista de Unidades na agenda de serviço</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>novo</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1 dia 6 horas atrás</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>11/03/2024</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>Petrolina-PE</t>
         </is>
@@ -19761,30 +19751,25 @@
           <t>[Petrolina-PE][Ambulatório] Sistema não agenda na data selecionada pela Solicitação de Procedimento de Serviço</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Filipe Carneiro</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1 dia 6 horas atrás</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4 dias 7 horas atrás</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
         <is>
           <t>Petrolina-PE</t>
         </is>
@@ -19799,30 +19784,25 @@
           <t>[Petrolina-PE][Regulação] Erro na negação de Unidade executante</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>aberto</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3 horas 5 minutos atrás</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5 dias 23 horas atrás</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>Petrolina-PE</t>
         </is>
@@ -19830,151 +19810,131 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>105678</v>
+        <v>108649</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[Volta Redonda-RJ][Hospital] Evolução do atendimento não salva</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>aberto</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>5</v>
+          <t>[Governador Valadares-MG][Hospital] - Pacientes internados no mesmo leito.</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>8 horas 9 minutos atrás</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>11/03/2024</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Volta Redonda-RJ</t>
+          <t>Governador Valadares-MG</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>105890</v>
+        <v>105678</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[Volta Redonda - RJ][Regulação] A função “Negação de procedimentos entre município solicitantes e municípios e unidades executantes” não está bloqueando as unidades parametrizadas</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>aberto</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>6</v>
+          <t>[Volta Redonda-RJ][Hospital] Evolução do atendimento não salva</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>11/03/2024</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>11/03/2024</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Volta Redonda - RJ</t>
+          <t>Volta Redonda-RJ</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>108918</v>
+        <v>105890</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[Governador Valadares-MG][Backup] - Oficio para disponibilização do backup dos dados da Saúde</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>aberto</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>7</v>
+          <t>[Volta Redonda - RJ][Regulação] A função “Negação de procedimentos entre município solicitantes e municípios e unidades executantes” não está bloqueando as unidades parametrizadas</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3 horas 1 minuto atrás</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>11/03/2024</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Governador Valadares-MG</t>
+          <t>Volta Redonda - RJ</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>108332</v>
+        <v>108729</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[Volta Redonda-RJ][Almoxarifado][Movimentação Consolidada de Produtos] Valores do relatório divergem</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>aberto</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>8</v>
+          <t>[Volta Redonda-RJ][Ambulatório][Exportação de Produção RAAS] Dados do Tipo de Gestão está incorreto no arquivo RAAS (Gestão Municipal)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1 dia 6 horas atrás</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6 dias 2 horas atrás</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
-        <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
         <is>
           <t>Volta Redonda-RJ</t>
         </is>
@@ -19982,115 +19942,100 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>108529</v>
+        <v>108918</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[São Luis- MA] [APP CIDADÃO] Melhoria no APP - REGULAÇÃO</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>aberto</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>9</v>
+          <t>[Governador Valadares-MG][Backup] - Oficio para disponibilização do backup dos dados da Saúde</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>11/03/2024</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4 dias 9 horas atrás</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>São Luis- MA</t>
+          <t>Governador Valadares-MG</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>108649</v>
+        <v>108332</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[Governador Valadares-MG][Hospital] - Pacientes internados no mesmo leito.</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Feedback</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>3</v>
+          <t>[Volta Redonda-RJ][Almoxarifado][Movimentação Consolidada de Produtos] Valores do relatório divergem</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>8 horas 48 minutos atrás</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5 dias 5 horas atrás</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Governador Valadares-MG</t>
+          <t>Volta Redonda-RJ</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>108729</v>
+        <v>108529</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[Volta Redonda-RJ][Ambulatório][Exportação de Produção RAAS] Dados do Tipo de Gestão está incorreto no arquivo RAAS (Gestão Municipal)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Filipe Carneiro</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>4</v>
+          <t>[São Luis- MA] [APP CIDADÃO] Melhoria no APP - REGULAÇÃO</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15/03/2024</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6 dias atrás</t>
+          <t>22/03/2024</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>19/03/2024</t>
+          <t>18:28:05</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>17:58:53</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Volta Redonda-RJ</t>
+          <t>São Luis- MA</t>
         </is>
       </c>
     </row>

</xml_diff>